<commit_message>
add result graph in exl file
</commit_message>
<xml_diff>
--- a/doc/movisign.xlsx
+++ b/doc/movisign.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19440" windowHeight="12240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -75,12 +75,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -120,11 +114,612 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Error Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.8899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7799999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1099999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8900000000000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>false positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$11:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.3500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5599999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1032</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>false negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$11:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0699999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="98157696"/>
+        <c:axId val="98083200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98157696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98083200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98083200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98157696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Error Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.3200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7800000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13739999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>false positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$18:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>false negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.2700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9799999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="98284288"/>
+        <c:axId val="98124160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98284288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98124160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98124160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98284288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="圖表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="圖表 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,14 +1041,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -670,7 +1265,7 @@
         <v>7.0699999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -933,10 +1528,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>